<commit_message>
update before final push
</commit_message>
<xml_diff>
--- a/Experiments/FogBench/results/final-results1.xlsx
+++ b/Experiments/FogBench/results/final-results1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcch\Documents\csc4006Gitlab\csc4006-EdgeBenchmarking\Experiments\FogBench\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC3A953-2677-466F-9318-9D610E36AD21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ED1117-D489-4AB6-818E-FC2F0D02E902}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{0EA3D584-B042-48D8-8859-F31D722D4D3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{0EA3D584-B042-48D8-8859-F31D722D4D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="iPokeMon Stress JMeter" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1447,7 +1446,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1502,7 +1501,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3075,6 +3074,31 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Concurrent Users</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3170,6 +3194,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Computation Latency (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3257,7 +3306,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3923,7 +3972,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Concurrent Users/Benchmarks</a:t>
+                  <a:t>Concurrent Users</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4135,7 +4184,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4196,6 +4245,1760 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Yolo (Odroid)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$3,'Multiple Users'!$O$6,'Multiple Users'!$O$9,'Multiple Users'!$O$12,'Multiple Users'!$O$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.5242767333333336</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5712492166666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8418728999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6339948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7481563000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Yolo (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$4,'Multiple Users'!$O$7,'Multiple Users'!$O$10,'Multiple Users'!$O$13,'Multiple Users'!$O$16)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.4558469333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5178091833333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7253124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8956426</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7278131000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Pocket Sphinx (Odroid XU4)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$18,'Multiple Users'!$O$21,'Multiple Users'!$O$24,'Multiple Users'!$O$27,'Multiple Users'!$O$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.5746129666666664</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6597779166666671</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5140202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2537929000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0834239000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Pocket Sphinx (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$19,'Multiple Users'!$O$22,'Multiple Users'!$O$25,'Multiple Users'!$O$28,'Multiple Users'!$O$31)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.6511803666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6824455999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5317718999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3518368999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6100137999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Aeneas (Odroid XU4)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$33,'Multiple Users'!$O$36,'Multiple Users'!$O$39,'Multiple Users'!$O$42,'Multiple Users'!$O$45)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.5190075333333302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7458752333333329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9237269000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3517777</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4018830000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Aeneas (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$34,'Multiple Users'!$O$37,'Multiple Users'!$O$40,'Multiple Users'!$O$43,'Multiple Users'!$O$46)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.7689746</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.731196133333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1491951</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1056313000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8796059000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>FogLamp (Odroid XU4)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$48,'Multiple Users'!$O$51,'Multiple Users'!$O$54,'Multiple Users'!$O$57,'Multiple Users'!$O$60)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.1444335800000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9952155799999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1128266999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4945110000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0987833999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>FogLamp (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$O$49,'Multiple Users'!$O$52,'Multiple Users'!$O$55,'Multiple Users'!$O$58,'Multiple Users'!$O$61)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.4567444599999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1511195000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2259764999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5402695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0242646</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-B9FF-4263-A30F-6015969D1196}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="424334528"/>
+        <c:axId val="424334200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="424334528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Concurrent Users</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424334200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="424334200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Computation Latency (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424334528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Yolo (Odroid)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$3,'Multiple Users'!$E$6,'Multiple Users'!$E$9,'Multiple Users'!$E$12,'Multiple Users'!$E$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14.238726325333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.022071098333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.936866317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.446972431999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.429608817999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Yolo (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$4,'Multiple Users'!$E$7,'Multiple Users'!$E$10,'Multiple Users'!$E$13,'Multiple Users'!$E$16)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40.150709158000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.699499764000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.465425107000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.945494003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.162775929999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Pocket Sphinx (Odroid XU4)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$18,'Multiple Users'!$E$21,'Multiple Users'!$E$24,'Multiple Users'!$E$27,'Multiple Users'!$E$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14.317428041999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.204612573333335</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.742338537999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.641699822</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.961913776999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Pocket Sphinx (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$19,'Multiple Users'!$E$22,'Multiple Users'!$E$25,'Multiple Users'!$E$28,'Multiple Users'!$E$31)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23.742193651000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.472721333999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.212797094999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.879375586000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.62327346</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Aeneas (Odroid XU4)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$33,'Multiple Users'!$E$36,'Multiple Users'!$E$39,'Multiple Users'!$E$42,'Multiple Users'!$E$45)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.3143515443333298</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8790910563333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.4661910169999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.443887875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.819436236000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Aeneas (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$34,'Multiple Users'!$E$37,'Multiple Users'!$E$40,'Multiple Users'!$E$43,'Multiple Users'!$E$46)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.6852877553333325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9206715209999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.196275848000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.845876101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.761265005999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>FogLamp (Odroid XU4)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$48,'Multiple Users'!$E$51,'Multiple Users'!$E$54,'Multiple Users'!$E$57,'Multiple Users'!$E$60)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.1979498999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1180344897000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1971966850000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.078875107</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.200035883</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>FogLamp (Raspberry Pi 3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Multiple Users'!$E$49,'Multiple Users'!$E$52,'Multiple Users'!$E$55,'Multiple Users'!$E$58,'Multiple Users'!$E$61)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.5452204650000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2157660340000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3224673189999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.654813962</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1458731439999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D52A-4BCF-8BB0-0AF16BD72C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="424334528"/>
+        <c:axId val="424334200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="424334528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Concurrent Users</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424334200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="424334200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Communication Latency (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424334528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4619,7 +6422,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4679,7 +6482,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5089,7 +6892,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5798,7 +7601,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -8609,7 +10412,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1100"/>
                   <a:t>Workload Stress Induced</a:t>
                 </a:r>
               </a:p>
@@ -8729,7 +10532,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1100"/>
                   <a:t>Communication Latency (sec)</a:t>
                 </a:r>
               </a:p>
@@ -8822,7 +10625,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -9474,7 +11277,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1100"/>
                   <a:t>Workload Stress Induced</a:t>
                 </a:r>
               </a:p>
@@ -9594,7 +11397,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1100"/>
                   <a:t>Communication Latency (sec)</a:t>
                 </a:r>
               </a:p>
@@ -9687,7 +11490,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -11557,7 +13360,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -12841,6 +14644,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -15174,7 +17057,7 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -15282,11 +17165,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -15297,11 +17175,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -15333,9 +17206,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -15690,7 +17560,7 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -15798,11 +17668,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -15813,11 +17678,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -15849,9 +17709,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -16205,8 +18062,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -16314,6 +18171,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -16324,6 +18186,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -16355,6 +18222,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -16708,8 +18578,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -16817,6 +18687,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -16827,6 +18702,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -16858,6 +18738,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -17211,8 +19094,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -17714,7 +19597,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18217,7 +20100,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18720,7 +20603,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19223,7 +21106,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19726,8 +21609,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -20229,18 +22112,1024 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>468279</xdr:colOff>
+      <xdr:colOff>544479</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
@@ -20697,6 +23586,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F27E4F5-C0B3-46AB-A7BF-1AE14E666F60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>14568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>600636</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>166968</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AF6884-8827-4176-86E2-A18EE8A21C47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -21083,8 +24048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317A88CD-561D-4524-8FFB-5C22E6F39745}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22608,8 +25573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642B8997-9E89-4E25-9612-C3B50DFEBD19}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AU30" sqref="AU30"/>
+    <sheetView topLeftCell="U19" workbookViewId="0">
+      <selection activeCell="AE42" sqref="AE42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24801,8 +27766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6FB09A-C09B-44CD-BC53-42A50E645BD9}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AX13" sqref="AX13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28232,7 +31197,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28978,8 +31943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027112F-048E-4E9B-927C-7ACA92AB6698}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>